<commit_message>
dpv-tech: reorganise into modules ; update DPV
- The DPV-TECH files and HTML have been reorganised into modules with
  distinctions between different categories of concepts
- The DPV concepts have been updated from spreadsheet
- Note: this does not contain the changelog or version change info
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/context_status.xlsx
+++ b/documentation-generator/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="280">
   <si>
     <t>Term</t>
   </si>
@@ -223,12 +223,18 @@
     <t>SporadicFrequency</t>
   </si>
   <si>
+    <t>Sporadic Frequency</t>
+  </si>
+  <si>
     <t>Frequency where occurences are sporadic or infrequent or sparse</t>
   </si>
   <si>
     <t>SingularFrequency</t>
   </si>
   <si>
+    <t>Singular Frequency</t>
+  </si>
+  <si>
     <t>Frequency where occurences are singular i.e. they take place only once</t>
   </si>
   <si>
@@ -238,10 +244,10 @@
     <t>The duration or temporal limitation</t>
   </si>
   <si>
-    <t>IndefiniteDuration</t>
-  </si>
-  <si>
-    <t>Indefinite Duration</t>
+    <t>IndeterminateDuration</t>
+  </si>
+  <si>
+    <t>Indeterminate Duration</t>
   </si>
   <si>
     <t>Duration that is indeterminate or cannot be determined</t>
@@ -259,30 +265,45 @@
     <t>EndlessDuration</t>
   </si>
   <si>
-    <t>Duration that is open ended or without an end</t>
+    <t>Endless Duration</t>
+  </si>
+  <si>
+    <t>Duration that is (known or intended to be) open ended or without an end</t>
   </si>
   <si>
     <t>TemporalDuration</t>
   </si>
   <si>
+    <t>Temporal Duration</t>
+  </si>
+  <si>
     <t>Duration that has a fixed temporal duration e.g. 6 months</t>
   </si>
   <si>
     <t>UntilEventDuration</t>
   </si>
   <si>
+    <t>Until Event Duration</t>
+  </si>
+  <si>
     <t>Duration that takes place until a specific event occurs e.g. Account Closure</t>
   </si>
   <si>
     <t>UntilTimeDuration</t>
   </si>
   <si>
+    <t>Until Time Duration</t>
+  </si>
+  <si>
     <t>Duration that has a fixed end date e.g. 2022-12-31</t>
   </si>
   <si>
     <t>FixedOccurencesDuration</t>
   </si>
   <si>
+    <t>Fixed Occurences Duration</t>
+  </si>
+  <si>
     <t>Duration that takes place a fixed number of times e.g. 3 times</t>
   </si>
   <si>
@@ -292,7 +313,7 @@
     <t>Purpose Duration</t>
   </si>
   <si>
-    <t>The duration associated with fulfilment or carrying out a purpose</t>
+    <t>The duration associated with fulfilment or carrying out purpose(s)</t>
   </si>
   <si>
     <t>Harshvardhan J. Pandit, Piero Bonatti</t>
@@ -304,7 +325,7 @@
     <t>Consent Duration</t>
   </si>
   <si>
-    <t>The duration associated with fulfilment or validity of a consenting decision</t>
+    <t>The duration associated with fulfilment or validity of consenting decision(s)</t>
   </si>
   <si>
     <t>ContractDuration</t>
@@ -313,7 +334,7 @@
     <t>Contract Duration</t>
   </si>
   <si>
-    <t>The duration associated with fulfilment or carrying out a contract</t>
+    <t>The duration associated with fulfilment or carrying out contract(s)</t>
   </si>
   <si>
     <t>domain</t>
@@ -501,7 +522,7 @@
     <t>is applicable for</t>
   </si>
   <si>
-    <t>Indicates applicability for specified context</t>
+    <t>Indicates applicability for specified context or criteria</t>
   </si>
   <si>
     <t>Harshvardhan J Pandit, Beatriz Esteves, Georg P Krog, Paul Ryan</t>
@@ -513,7 +534,7 @@
     <t>is not applicable for</t>
   </si>
   <si>
-    <t>Indicates non-applicability for specified context</t>
+    <t>Indicates non-applicability for specified context or criteria</t>
   </si>
   <si>
     <t>The status or state of something</t>
@@ -675,6 +696,9 @@
     <t>State of being unlawful or legally non-compliant</t>
   </si>
   <si>
+    <t>LawfulnessUnkown</t>
+  </si>
+  <si>
     <t>GDPR specific statuses in dpv-gdpr</t>
   </si>
   <si>
@@ -705,6 +729,9 @@
     <t>State of being unlawful or legally non-compliant for GDPR</t>
   </si>
   <si>
+    <t>GDPRComplianceUnknown</t>
+  </si>
+  <si>
     <t>AuditStatus</t>
   </si>
   <si>
@@ -778,6 +805,15 @@
   </si>
   <si>
     <t>State where an audit is determined as being required but has not been conducted</t>
+  </si>
+  <si>
+    <t>ConformanceStatus</t>
+  </si>
+  <si>
+    <t>Conformant</t>
+  </si>
+  <si>
+    <t>NonConformant</t>
   </si>
   <si>
     <t>hasStatus</t>
@@ -2318,10 +2354,10 @@
         <v>68</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>64</v>
@@ -2367,13 +2403,13 @@
     </row>
     <row r="22">
       <c r="A22" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>64</v>
@@ -2430,13 +2466,13 @@
     </row>
     <row r="24">
       <c r="A24" s="15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>24</v>
@@ -2480,16 +2516,16 @@
     </row>
     <row r="25">
       <c r="A25" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>18</v>
@@ -2498,13 +2534,13 @@
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
       <c r="M25" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
@@ -2524,16 +2560,16 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>18</v>
@@ -2576,16 +2612,16 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>25</v>
@@ -2628,16 +2664,16 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>25</v>
@@ -2680,16 +2716,16 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>25</v>
@@ -2732,16 +2768,16 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>25</v>
@@ -2784,16 +2820,16 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>25</v>
@@ -2806,10 +2842,10 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
       <c r="M31" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
@@ -2828,16 +2864,16 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>25</v>
@@ -2850,10 +2886,10 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O32" s="11"/>
       <c r="P32" s="11"/>
@@ -2872,16 +2908,16 @@
     </row>
     <row r="33">
       <c r="A33" s="12" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>25</v>
@@ -2894,10 +2930,10 @@
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
       <c r="M33" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N33" s="12" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O33" s="11"/>
       <c r="P33" s="11"/>
@@ -5543,13 +5579,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -5564,7 +5600,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -5581,13 +5617,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -5596,7 +5632,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -5631,27 +5667,27 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="12" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="17">
@@ -5664,7 +5700,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="O3" s="19" t="s">
         <v>52</v>
@@ -5687,28 +5723,28 @@
     </row>
     <row r="4">
       <c r="A4" s="29" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D4" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G4" s="31"/>
       <c r="H4" s="31"/>
       <c r="I4" s="31"/>
       <c r="J4" s="32" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="K4" s="33">
         <v>43560.0</v>
@@ -5718,7 +5754,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="35" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="O4" s="36" t="s">
         <v>21</v>
@@ -5741,13 +5777,13 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D5" s="39" t="s">
         <v>17</v>
@@ -5756,7 +5792,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
@@ -5770,10 +5806,10 @@
         <v>27</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="O5" s="43" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="P5" s="44"/>
       <c r="Q5" s="44"/>
@@ -5793,13 +5829,13 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
@@ -5808,7 +5844,7 @@
         <v>64</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -5825,7 +5861,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -5845,13 +5881,13 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D7" s="45" t="s">
         <v>17</v>
@@ -5860,7 +5896,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -5874,10 +5910,10 @@
         <v>27</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -5897,13 +5933,13 @@
     </row>
     <row r="8">
       <c r="A8" s="12" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D8" s="45" t="s">
         <v>17</v>
@@ -5912,7 +5948,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="45" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
@@ -5926,10 +5962,10 @@
         <v>27</v>
       </c>
       <c r="N8" s="46" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="11"/>
@@ -5949,22 +5985,22 @@
     </row>
     <row r="9">
       <c r="A9" s="12" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
@@ -6001,22 +6037,22 @@
     </row>
     <row r="10">
       <c r="A10" s="12" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
@@ -6053,13 +6089,13 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>17</v>
@@ -6068,7 +6104,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
@@ -6085,7 +6121,7 @@
         <v>51</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -6105,27 +6141,27 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="12" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="17">
@@ -6135,10 +6171,10 @@
         <v>44727.0</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="O12" s="19" t="s">
         <v>55</v>
@@ -6161,13 +6197,13 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>17</v>
@@ -6176,7 +6212,7 @@
         <v>17</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
@@ -6185,10 +6221,10 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
@@ -6209,13 +6245,13 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C14" s="47" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>17</v>
@@ -6224,7 +6260,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
@@ -6233,10 +6269,10 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
       <c r="M14" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
@@ -9348,7 +9384,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>24</v>
@@ -9372,7 +9408,7 @@
         <v>51</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -9404,16 +9440,16 @@
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>25</v>
@@ -9434,7 +9470,7 @@
         <v>51</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -9454,16 +9490,16 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>18</v>
@@ -9484,7 +9520,7 @@
         <v>51</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -9504,16 +9540,16 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>18</v>
@@ -9534,7 +9570,7 @@
         <v>51</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="11"/>
@@ -9554,16 +9590,16 @@
     </row>
     <row r="7">
       <c r="A7" s="12" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>18</v>
@@ -9584,7 +9620,7 @@
         <v>51</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -9604,16 +9640,16 @@
     </row>
     <row r="8">
       <c r="A8" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>170</v>
       </c>
       <c r="E8" s="49" t="s">
         <v>18</v>
@@ -9634,7 +9670,7 @@
         <v>51</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P8" s="51"/>
       <c r="Q8" s="51"/>
@@ -9666,16 +9702,16 @@
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>25</v>
@@ -9696,7 +9732,7 @@
         <v>51</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -9716,16 +9752,16 @@
     </row>
     <row r="11">
       <c r="A11" s="12" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>18</v>
@@ -9746,7 +9782,7 @@
         <v>51</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P11" s="11"/>
       <c r="Q11" s="11"/>
@@ -9766,16 +9802,16 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>18</v>
@@ -9784,7 +9820,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="12" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="17">
@@ -9792,13 +9828,13 @@
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="12" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>51</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
@@ -9818,16 +9854,16 @@
     </row>
     <row r="13">
       <c r="A13" s="12" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C13" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>192</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>185</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>18</v>
@@ -9848,7 +9884,7 @@
         <v>51</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
@@ -9868,16 +9904,16 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>18</v>
@@ -9886,7 +9922,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="12" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="17">
@@ -9896,13 +9932,13 @@
         <v>44811.0</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>51</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -9922,16 +9958,16 @@
     </row>
     <row r="15">
       <c r="A15" s="12" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>18</v>
@@ -9940,7 +9976,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="12" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="17">
@@ -9950,13 +9986,13 @@
         <v>44811.0</v>
       </c>
       <c r="M15" s="12" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="N15" s="12" t="s">
         <v>51</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P15" s="11"/>
       <c r="Q15" s="11"/>
@@ -9976,16 +10012,16 @@
     </row>
     <row r="16">
       <c r="A16" s="12" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>18</v>
@@ -10024,16 +10060,16 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>18</v>
@@ -10080,16 +10116,16 @@
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>25</v>
@@ -10102,7 +10138,7 @@
       <c r="K19" s="11"/>
       <c r="L19" s="11"/>
       <c r="M19" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
@@ -10124,16 +10160,16 @@
     </row>
     <row r="20">
       <c r="A20" s="12" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>18</v>
@@ -10146,7 +10182,7 @@
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
       <c r="M20" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
@@ -10168,16 +10204,16 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>18</v>
@@ -10190,7 +10226,7 @@
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
       <c r="M21" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
@@ -10211,101 +10247,171 @@
       <c r="AD21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="52" t="s">
-        <v>215</v>
-      </c>
+      <c r="A22" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="11"/>
+      <c r="Y22" s="11"/>
+      <c r="Z22" s="11"/>
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="11"/>
+      <c r="AC22" s="11"/>
+      <c r="AD22" s="11"/>
     </row>
     <row r="23">
-      <c r="A23" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="A23" s="52"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24">
-      <c r="A24" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>221</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="A24" s="52" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25">
       <c r="A25" s="12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="20"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="11"/>
+      <c r="Z26" s="11"/>
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="11"/>
+      <c r="AC26" s="11"/>
+      <c r="AD26" s="11"/>
     </row>
     <row r="27">
-      <c r="A27" s="15" t="s">
-        <v>225</v>
+      <c r="A27" s="12" t="s">
+        <v>230</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>166</v>
+        <v>232</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
-      <c r="K27" s="17">
-        <v>44699.0</v>
-      </c>
+      <c r="K27" s="11"/>
       <c r="L27" s="11"/>
       <c r="M27" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O27" s="19" t="s">
-        <v>147</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
       <c r="R27" s="11"/>
@@ -10324,38 +10430,24 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>18</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
-      <c r="K28" s="17">
-        <v>44699.0</v>
-      </c>
+      <c r="K28" s="11"/>
       <c r="L28" s="11"/>
       <c r="M28" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O28" s="19" t="s">
-        <v>147</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="11"/>
       <c r="R28" s="11"/>
@@ -10373,72 +10465,23 @@
       <c r="AD28" s="11"/>
     </row>
     <row r="29">
-      <c r="A29" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>233</v>
-      </c>
-      <c r="C29" s="12" t="s">
+      <c r="B29" s="20"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="17">
-        <v>44741.0</v>
-      </c>
-      <c r="L29" s="11"/>
-      <c r="M29" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N29" s="12" t="s">
+      <c r="C30" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="O29" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
-      <c r="AB29" s="11"/>
-      <c r="AC29" s="11"/>
-      <c r="AD29" s="11"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>231</v>
+      <c r="D30" s="45" t="s">
+        <v>173</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -10456,7 +10499,7 @@
         <v>51</v>
       </c>
       <c r="O30" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P30" s="11"/>
       <c r="Q30" s="11"/>
@@ -10476,16 +10519,16 @@
     </row>
     <row r="31">
       <c r="A31" s="12" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>18</v>
@@ -10506,7 +10549,7 @@
         <v>51</v>
       </c>
       <c r="O31" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P31" s="11"/>
       <c r="Q31" s="11"/>
@@ -10526,16 +10569,16 @@
     </row>
     <row r="32">
       <c r="A32" s="12" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>18</v>
@@ -10543,20 +10586,22 @@
       <c r="F32" s="11"/>
       <c r="G32" s="11"/>
       <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
+      <c r="I32" s="12" t="s">
+        <v>244</v>
+      </c>
       <c r="J32" s="11"/>
       <c r="K32" s="17">
-        <v>44699.0</v>
+        <v>44741.0</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="12" t="s">
         <v>27</v>
       </c>
       <c r="N32" s="12" t="s">
-        <v>51</v>
+        <v>245</v>
       </c>
       <c r="O32" s="19" t="s">
-        <v>147</v>
+        <v>246</v>
       </c>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -10585,7 +10630,7 @@
         <v>249</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>18</v>
@@ -10606,7 +10651,7 @@
         <v>51</v>
       </c>
       <c r="O33" s="19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P33" s="11"/>
       <c r="Q33" s="11"/>
@@ -10625,24 +10670,174 @@
       <c r="AD33" s="11"/>
     </row>
     <row r="34">
-      <c r="B34" s="20"/>
+      <c r="A34" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L34" s="11"/>
+      <c r="M34" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O34" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="11"/>
+      <c r="Z34" s="11"/>
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
     </row>
     <row r="35">
-      <c r="B35" s="20"/>
+      <c r="A35" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O35" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
     </row>
     <row r="36">
-      <c r="B36" s="20"/>
+      <c r="A36" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L36" s="11"/>
+      <c r="M36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N36" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O36" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+      <c r="Y36" s="11"/>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="11"/>
+      <c r="AC36" s="11"/>
+      <c r="AD36" s="11"/>
     </row>
     <row r="37">
       <c r="B37" s="20"/>
     </row>
     <row r="38">
+      <c r="A38" s="15" t="s">
+        <v>259</v>
+      </c>
       <c r="B38" s="20"/>
     </row>
     <row r="39">
+      <c r="A39" s="12" t="s">
+        <v>260</v>
+      </c>
       <c r="B39" s="20"/>
     </row>
     <row r="40">
+      <c r="A40" s="12" t="s">
+        <v>261</v>
+      </c>
       <c r="B40" s="20"/>
     </row>
     <row r="41">
@@ -13144,23 +13339,32 @@
     <row r="873">
       <c r="B873" s="20"/>
     </row>
+    <row r="874">
+      <c r="B874" s="20"/>
+    </row>
+    <row r="875">
+      <c r="B875" s="20"/>
+    </row>
+    <row r="876">
+      <c r="B876" s="20"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:AD196">
+  <conditionalFormatting sqref="A2:AD199">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AD75">
+  <conditionalFormatting sqref="A2:AD78">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N195 AC2:AD195 A11:L195 O11:AB195">
+  <conditionalFormatting sqref="M2:N198 AC2:AD198 A11:L198 O11:AB198">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N195 AC2:AD195 A11:L195 O11:AB195">
+  <conditionalFormatting sqref="M2:N198 AC2:AD198 A11:L198 O11:AB198">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
@@ -13178,13 +13382,13 @@
     <hyperlink r:id="rId10" ref="O13"/>
     <hyperlink r:id="rId11" ref="O14"/>
     <hyperlink r:id="rId12" ref="O15"/>
-    <hyperlink r:id="rId13" ref="O27"/>
-    <hyperlink r:id="rId14" ref="O28"/>
-    <hyperlink r:id="rId15" ref="O29"/>
-    <hyperlink r:id="rId16" ref="O30"/>
-    <hyperlink r:id="rId17" ref="O31"/>
-    <hyperlink r:id="rId18" ref="O32"/>
-    <hyperlink r:id="rId19" ref="O33"/>
+    <hyperlink r:id="rId13" ref="O30"/>
+    <hyperlink r:id="rId14" ref="O31"/>
+    <hyperlink r:id="rId15" ref="O32"/>
+    <hyperlink r:id="rId16" ref="O33"/>
+    <hyperlink r:id="rId17" ref="O34"/>
+    <hyperlink r:id="rId18" ref="O35"/>
+    <hyperlink r:id="rId19" ref="O36"/>
   </hyperlinks>
   <drawing r:id="rId20"/>
 </worksheet>
@@ -13220,13 +13424,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="G1" s="21" t="s">
         <v>6</v>
@@ -13241,7 +13445,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="L1" s="26" t="s">
         <v>11</v>
@@ -13258,22 +13462,22 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
@@ -13290,7 +13494,7 @@
         <v>51</v>
       </c>
       <c r="O2" s="16" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
@@ -13308,22 +13512,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -13340,7 +13544,7 @@
         <v>51</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
@@ -13358,22 +13562,22 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -13390,7 +13594,7 @@
         <v>51</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -13408,22 +13612,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -13440,7 +13644,7 @@
         <v>51</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -13458,22 +13662,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -13482,7 +13686,7 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>

</xml_diff>

<commit_message>
adds DPIA properties, updates concepts, fixes bugs
- The DPIA properties are added in CSV, RDF, and HTML
- Concept updates from spreadsheets have been incorporated (note there
  is no corresponding changelog generated)
- bugs have been fixed related to use of older rdflib methods
  (graph.parse replaces graph.load)
- This commit also serves to demonstrate the use of external properties
  (added in previous commit) through the DPIA section in DPV-GDPR
</commit_message>
<xml_diff>
--- a/documentation-generator/vocab_csv/context_status.xlsx
+++ b/documentation-generator/vocab_csv/context_status.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="315">
   <si>
     <t>Term</t>
   </si>
@@ -591,6 +591,18 @@
     <t>State of an activity that has completed i.e. is fully in the past</t>
   </si>
   <si>
+    <t>ActivityNotCompleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acitivity Not Completed </t>
+  </si>
+  <si>
+    <t>State of an activity that could not be completed, but has reached some end state</t>
+  </si>
+  <si>
+    <t>This relates to a 'Stop' state as distinct from a 'Halt' state. It makes no comments on whether the Acitivity can be resumed or continued towards completion.</t>
+  </si>
+  <si>
     <t>ComplianceStatus</t>
   </si>
   <si>
@@ -681,6 +693,9 @@
     <t>Status associated with being lawful</t>
   </si>
   <si>
+    <t>https://www.w3.org/2022/10/19-dpvcg-minutes.html</t>
+  </si>
+  <si>
     <t>Lawful</t>
   </si>
   <si>
@@ -802,6 +817,108 @@
   </si>
   <si>
     <t>State of being non-conformant</t>
+  </si>
+  <si>
+    <t>RequestStatus</t>
+  </si>
+  <si>
+    <t>Request Status</t>
+  </si>
+  <si>
+    <t>Status associated with requests</t>
+  </si>
+  <si>
+    <t>RequestInitiated</t>
+  </si>
+  <si>
+    <t>Request Initiated</t>
+  </si>
+  <si>
+    <t>State of a request being initiated</t>
+  </si>
+  <si>
+    <t>dpv:RequestStatus</t>
+  </si>
+  <si>
+    <t>RequestAcknowledged</t>
+  </si>
+  <si>
+    <t>Request Acknowledged</t>
+  </si>
+  <si>
+    <t>State of a request being acknowledged</t>
+  </si>
+  <si>
+    <t>RequestAccepted</t>
+  </si>
+  <si>
+    <t>Request Accepted</t>
+  </si>
+  <si>
+    <t>State of a request being accepted towards fulfilment</t>
+  </si>
+  <si>
+    <t>RequestRejected</t>
+  </si>
+  <si>
+    <t>Request Rejected</t>
+  </si>
+  <si>
+    <t>State of a request being rejected towards non-fulfilment</t>
+  </si>
+  <si>
+    <t>RequestFulfilled</t>
+  </si>
+  <si>
+    <t>Request Fulfilled</t>
+  </si>
+  <si>
+    <t>State of a request being fulfilled</t>
+  </si>
+  <si>
+    <t>RequestUnfulfilled</t>
+  </si>
+  <si>
+    <t>Request Unfulfilled</t>
+  </si>
+  <si>
+    <t>State of a request being unfulfilled</t>
+  </si>
+  <si>
+    <t>RequestRequiresAction</t>
+  </si>
+  <si>
+    <t>Request Requires Action</t>
+  </si>
+  <si>
+    <t>State of a request requiring an action to be performed from another party</t>
+  </si>
+  <si>
+    <t>RequestRequiredActionPerformed</t>
+  </si>
+  <si>
+    <t>Request Required Action Performed</t>
+  </si>
+  <si>
+    <t>State of a request's required action having been performed by the other party</t>
+  </si>
+  <si>
+    <t>RequestActionDelayed</t>
+  </si>
+  <si>
+    <t>Request Action Delayed</t>
+  </si>
+  <si>
+    <t>State of a request being delayed towards fulfilment</t>
+  </si>
+  <si>
+    <t>RequestStatusQuery</t>
+  </si>
+  <si>
+    <t>Request Status Query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State of a request's status being queried </t>
   </si>
   <si>
     <t>hasStatus</t>
@@ -1043,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1183,6 +1300,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -6194,7 +6314,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>114</v>
@@ -6242,7 +6362,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>114</v>
@@ -6280,9 +6400,11 @@
       <c r="B15" s="20"/>
     </row>
     <row r="16">
+      <c r="A16" s="48"/>
       <c r="B16" s="20"/>
     </row>
     <row r="17">
+      <c r="A17" s="48"/>
       <c r="B17" s="20"/>
     </row>
     <row r="18">
@@ -9593,7 +9715,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
-      <c r="J7" s="48"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="17">
         <v>44699.0</v>
       </c>
@@ -9624,25 +9746,25 @@
       <c r="AD7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="50" t="s">
         <v>186</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
       <c r="J8" s="11"/>
       <c r="K8" s="17">
         <v>44699.0</v>
@@ -9657,99 +9779,95 @@
       <c r="O8" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Y8" s="51"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="52"/>
+      <c r="T8" s="52"/>
+      <c r="U8" s="52"/>
+      <c r="V8" s="52"/>
+      <c r="W8" s="52"/>
+      <c r="X8" s="52"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="52"/>
+      <c r="AA8" s="52"/>
+      <c r="AB8" s="52"/>
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="12"/>
+      <c r="A9" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>177</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="J9" s="11"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="N9" s="12"/>
       <c r="O9" s="18"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="11"/>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="11"/>
+      <c r="AC9" s="11"/>
+      <c r="AD9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="D10" s="45" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="12"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E11" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="17">
-        <v>44699.0</v>
-      </c>
-      <c r="L10" s="17"/>
-      <c r="M10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O10" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -9759,7 +9877,7 @@
       <c r="K11" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="17"/>
       <c r="M11" s="12" t="s">
         <v>27</v>
       </c>
@@ -9787,16 +9905,16 @@
     </row>
     <row r="12">
       <c r="A12" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>18</v>
@@ -9804,16 +9922,14 @@
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
-      <c r="I12" s="12" t="s">
-        <v>195</v>
-      </c>
+      <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="17">
         <v>44699.0</v>
       </c>
       <c r="L12" s="11"/>
       <c r="M12" s="12" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>51</v>
@@ -9842,13 +9958,13 @@
         <v>197</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>199</v>
-      </c>
       <c r="D13" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>18</v>
@@ -9856,14 +9972,16 @@
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="I13" s="12" t="s">
+        <v>199</v>
+      </c>
       <c r="J13" s="11"/>
       <c r="K13" s="17">
         <v>44699.0</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="12" t="s">
-        <v>27</v>
+        <v>200</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>51</v>
@@ -9889,16 +10007,16 @@
     </row>
     <row r="14">
       <c r="A14" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>18</v>
@@ -9906,18 +10024,14 @@
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="12" t="s">
-        <v>203</v>
-      </c>
+      <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="17">
         <v>44699.0</v>
       </c>
-      <c r="L14" s="17">
-        <v>44811.0</v>
-      </c>
+      <c r="L14" s="11"/>
       <c r="M14" s="12" t="s">
-        <v>160</v>
+        <v>27</v>
       </c>
       <c r="N14" s="12" t="s">
         <v>51</v>
@@ -9952,7 +10066,7 @@
         <v>206</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>18</v>
@@ -10006,7 +10120,7 @@
         <v>210</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>18</v>
@@ -10014,19 +10128,25 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="12" t="s">
+        <v>211</v>
+      </c>
       <c r="J16" s="11"/>
       <c r="K16" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L16" s="17">
         <v>44811.0</v>
       </c>
-      <c r="L16" s="11"/>
       <c r="M16" s="12" t="s">
-        <v>27</v>
+        <v>160</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="O16" s="18"/>
+      <c r="O16" s="19" t="s">
+        <v>154</v>
+      </c>
       <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
@@ -10045,16 +10165,16 @@
     </row>
     <row r="17">
       <c r="A17" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>18</v>
@@ -10092,85 +10212,94 @@
       <c r="AD17" s="11"/>
     </row>
     <row r="18">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="M18" s="12"/>
+      <c r="A18" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="17">
+        <v>44811.0</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N18" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="18"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="11"/>
+      <c r="AC18" s="11"/>
+      <c r="AD18" s="11"/>
     </row>
     <row r="19">
-      <c r="A19" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="12" t="s">
-        <v>217</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
       <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="17">
+        <v>44853.0</v>
+      </c>
       <c r="L20" s="11"/>
       <c r="M20" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
+      <c r="N20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>221</v>
+      </c>
       <c r="P20" s="11"/>
       <c r="Q20" s="11"/>
       <c r="R20" s="11"/>
@@ -10189,16 +10318,16 @@
     </row>
     <row r="21">
       <c r="A21" s="12" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>18</v>
@@ -10208,13 +10337,19 @@
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="K21" s="14">
+        <v>44853.0</v>
+      </c>
       <c r="L21" s="11"/>
       <c r="M21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
+      <c r="N21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>221</v>
+      </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
       <c r="R21" s="11"/>
@@ -10232,17 +10367,17 @@
       <c r="AD21" s="11"/>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>223</v>
+      <c r="A22" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>219</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>18</v>
@@ -10252,13 +10387,19 @@
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="K22" s="14">
+        <v>44853.0</v>
+      </c>
       <c r="L22" s="11"/>
       <c r="M22" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
+      <c r="N22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>221</v>
+      </c>
       <c r="P22" s="11"/>
       <c r="Q22" s="11"/>
       <c r="R22" s="11"/>
@@ -10276,73 +10417,73 @@
       <c r="AD22" s="11"/>
     </row>
     <row r="23">
-      <c r="B23" s="20"/>
+      <c r="A23" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="14">
+        <v>44853.0</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11"/>
+      <c r="Z23" s="11"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
     </row>
     <row r="24">
-      <c r="A24" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="D24" s="45" t="s">
+      <c r="B24" s="20"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="17">
-        <v>44699.0</v>
-      </c>
-      <c r="L24" s="11"/>
-      <c r="M24" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O24" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
-      <c r="AB24" s="11"/>
-      <c r="AC24" s="11"/>
-      <c r="AD24" s="11"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -10380,16 +10521,16 @@
     </row>
     <row r="26">
       <c r="A26" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>18</v>
@@ -10397,22 +10538,20 @@
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
-      <c r="I26" s="12" t="s">
-        <v>235</v>
-      </c>
+      <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="17">
-        <v>44741.0</v>
+        <v>44699.0</v>
       </c>
       <c r="L26" s="11"/>
       <c r="M26" s="12" t="s">
         <v>27</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>236</v>
+        <v>51</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>237</v>
+        <v>154</v>
       </c>
       <c r="P26" s="11"/>
       <c r="Q26" s="11"/>
@@ -10432,16 +10571,16 @@
     </row>
     <row r="27">
       <c r="A27" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>240</v>
-      </c>
       <c r="D27" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>18</v>
@@ -10449,20 +10588,22 @@
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="I27" s="12" t="s">
+        <v>240</v>
+      </c>
       <c r="J27" s="11"/>
       <c r="K27" s="17">
-        <v>44699.0</v>
+        <v>44741.0</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="12" t="s">
         <v>27</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>51</v>
+        <v>241</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -10482,16 +10623,16 @@
     </row>
     <row r="28">
       <c r="A28" s="12" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>18</v>
@@ -10532,16 +10673,16 @@
     </row>
     <row r="29">
       <c r="A29" s="12" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>18</v>
@@ -10582,16 +10723,16 @@
     </row>
     <row r="30">
       <c r="A30" s="12" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>18</v>
@@ -10631,71 +10772,73 @@
       <c r="AD30" s="11"/>
     </row>
     <row r="31">
-      <c r="B31" s="20"/>
+      <c r="A31" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>253</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="17">
+        <v>44699.0</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O31" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+      <c r="Y31" s="11"/>
+      <c r="Z31" s="11"/>
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="11"/>
+      <c r="AD31" s="11"/>
     </row>
     <row r="32">
-      <c r="A32" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="B32" s="20"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E33" s="12" t="s">
         <v>25</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="17">
-        <v>44856.0</v>
-      </c>
-      <c r="L32" s="11"/>
-      <c r="M32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N32" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="11"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="11"/>
-      <c r="AB32" s="11"/>
-      <c r="AC32" s="11"/>
-      <c r="AD32" s="11"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -10731,16 +10874,16 @@
     </row>
     <row r="34">
       <c r="A34" s="12" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>18</v>
@@ -10778,45 +10921,564 @@
       <c r="AD34" s="11"/>
     </row>
     <row r="35">
-      <c r="B35" s="20"/>
+      <c r="A35" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="17">
+        <v>44856.0</v>
+      </c>
+      <c r="L35" s="11"/>
+      <c r="M35" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N35" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
     </row>
     <row r="36">
       <c r="B36" s="20"/>
     </row>
     <row r="37">
-      <c r="B37" s="20"/>
+      <c r="A37" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N37" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+      <c r="Y37" s="11"/>
+      <c r="Z37" s="11"/>
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="11"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
     </row>
     <row r="38">
-      <c r="B38" s="20"/>
+      <c r="A38" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="11"/>
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="11"/>
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="11"/>
     </row>
     <row r="39">
-      <c r="B39" s="20"/>
+      <c r="A39" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11"/>
+      <c r="AD39" s="11"/>
     </row>
     <row r="40">
-      <c r="B40" s="20"/>
+      <c r="A40" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N40" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+      <c r="Y40" s="11"/>
+      <c r="Z40" s="11"/>
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="11"/>
+      <c r="AC40" s="11"/>
+      <c r="AD40" s="11"/>
     </row>
     <row r="41">
-      <c r="B41" s="20"/>
+      <c r="A41" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N41" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+      <c r="Y41" s="11"/>
+      <c r="Z41" s="11"/>
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="11"/>
+      <c r="AC41" s="11"/>
+      <c r="AD41" s="11"/>
     </row>
     <row r="42">
-      <c r="B42" s="20"/>
+      <c r="A42" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N42" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
+      <c r="Z42" s="11"/>
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="11"/>
+      <c r="AC42" s="11"/>
+      <c r="AD42" s="11"/>
     </row>
     <row r="43">
-      <c r="B43" s="20"/>
+      <c r="A43" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N43" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+      <c r="Y43" s="11"/>
+      <c r="Z43" s="11"/>
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="11"/>
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="11"/>
     </row>
     <row r="44">
-      <c r="B44" s="20"/>
+      <c r="A44" s="12" t="s">
+        <v>285</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N44" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+      <c r="Y44" s="11"/>
+      <c r="Z44" s="11"/>
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="11"/>
+      <c r="AC44" s="11"/>
+      <c r="AD44" s="11"/>
     </row>
     <row r="45">
-      <c r="B45" s="20"/>
+      <c r="A45" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N45" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+      <c r="Y45" s="11"/>
+      <c r="Z45" s="11"/>
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="11"/>
+      <c r="AC45" s="11"/>
+      <c r="AD45" s="11"/>
     </row>
     <row r="46">
-      <c r="B46" s="20"/>
+      <c r="A46" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N46" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+      <c r="Y46" s="11"/>
+      <c r="Z46" s="11"/>
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="11"/>
+      <c r="AC46" s="11"/>
+      <c r="AD46" s="11"/>
     </row>
     <row r="47">
-      <c r="B47" s="20"/>
+      <c r="A47" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N47" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+      <c r="Z47" s="11"/>
+      <c r="AA47" s="11"/>
+      <c r="AB47" s="11"/>
+      <c r="AC47" s="11"/>
+      <c r="AD47" s="11"/>
     </row>
     <row r="48">
+      <c r="A48" s="12"/>
       <c r="B48" s="20"/>
     </row>
     <row r="49">
@@ -13296,12 +13958,12 @@
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N192 AC2:AD192 A11:L192 O11:AB192">
+  <conditionalFormatting sqref="M2:N192 AC2:AD192 A12:L192 O12:AB192">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:N192 AC2:AD192 A11:L192 O11:AB192">
+  <conditionalFormatting sqref="M2:N192 AC2:AD192 A12:L192 O12:AB192">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>$M2="deprecated"</formula>
     </cfRule>
@@ -13313,21 +13975,25 @@
     <hyperlink r:id="rId4" ref="O6"/>
     <hyperlink r:id="rId5" ref="O7"/>
     <hyperlink r:id="rId6" ref="O8"/>
-    <hyperlink r:id="rId7" ref="O10"/>
-    <hyperlink r:id="rId8" ref="O11"/>
-    <hyperlink r:id="rId9" ref="O12"/>
-    <hyperlink r:id="rId10" ref="O13"/>
-    <hyperlink r:id="rId11" ref="O14"/>
-    <hyperlink r:id="rId12" ref="O15"/>
-    <hyperlink r:id="rId13" ref="O24"/>
-    <hyperlink r:id="rId14" ref="O25"/>
-    <hyperlink r:id="rId15" ref="O26"/>
-    <hyperlink r:id="rId16" ref="O27"/>
-    <hyperlink r:id="rId17" ref="O28"/>
-    <hyperlink r:id="rId18" ref="O29"/>
-    <hyperlink r:id="rId19" ref="O30"/>
+    <hyperlink r:id="rId7" ref="O11"/>
+    <hyperlink r:id="rId8" ref="O12"/>
+    <hyperlink r:id="rId9" ref="O13"/>
+    <hyperlink r:id="rId10" ref="O14"/>
+    <hyperlink r:id="rId11" ref="O15"/>
+    <hyperlink r:id="rId12" ref="O16"/>
+    <hyperlink r:id="rId13" ref="O20"/>
+    <hyperlink r:id="rId14" ref="O21"/>
+    <hyperlink r:id="rId15" ref="O22"/>
+    <hyperlink r:id="rId16" ref="O23"/>
+    <hyperlink r:id="rId17" ref="O25"/>
+    <hyperlink r:id="rId18" ref="O26"/>
+    <hyperlink r:id="rId19" ref="O27"/>
+    <hyperlink r:id="rId20" ref="O28"/>
+    <hyperlink r:id="rId21" ref="O29"/>
+    <hyperlink r:id="rId22" ref="O30"/>
+    <hyperlink r:id="rId23" ref="O31"/>
   </hyperlinks>
-  <drawing r:id="rId20"/>
+  <drawing r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -13399,13 +14065,13 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>258</v>
+        <v>297</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>259</v>
+        <v>298</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>17</v>
@@ -13449,22 +14115,22 @@
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
-        <v>261</v>
+        <v>300</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>262</v>
+        <v>301</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -13499,13 +14165,13 @@
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
-        <v>265</v>
+        <v>304</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>266</v>
+        <v>305</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>17</v>
@@ -13514,7 +14180,7 @@
         <v>177</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -13549,22 +14215,22 @@
     </row>
     <row r="5">
       <c r="A5" s="12" t="s">
-        <v>268</v>
+        <v>307</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>270</v>
+        <v>309</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>264</v>
+        <v>303</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -13581,7 +14247,7 @@
         <v>51</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>271</v>
+        <v>310</v>
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="11"/>
@@ -13599,22 +14265,22 @@
     </row>
     <row r="6">
       <c r="A6" s="12" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>273</v>
+        <v>312</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>274</v>
+        <v>313</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>275</v>
+        <v>314</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>

</xml_diff>